<commit_message>
Fixed normalising of inhibition curve
</commit_message>
<xml_diff>
--- a/Example/Example.xlsx
+++ b/Example/Example.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="15180" windowHeight="9090"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="15180" windowHeight="9090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
+    <sheet name="Inhibition" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -900,7 +901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -1329,4 +1332,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>8450</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>0.3</v>
+      </c>
+      <c r="B2">
+        <v>11527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>10349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>9793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>6493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>9647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>300</v>
+      </c>
+      <c r="B9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>10023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>0.3</v>
+      </c>
+      <c r="B11">
+        <v>10946</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>9025</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>10467</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>9341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Linear eq introduced and tested: testLinear.py
</commit_message>
<xml_diff>
--- a/Example/Example.xlsx
+++ b/Example/Example.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="15180" windowHeight="9090" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="15180" windowHeight="9090" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Example" sheetId="1" r:id="rId1"/>
+    <sheet name="Dose_Resp" sheetId="1" r:id="rId1"/>
     <sheet name="Inhibition" sheetId="2" r:id="rId2"/>
+    <sheet name="Linear" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -543,74 +544,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -622,7 +555,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C0C0C0"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1338,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1460,4 +1393,99 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>14.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>11.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>25.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>13.81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>25.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>26.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>38.86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>